<commit_message>
Add updated template for StudentClass, VocationalTrainer, VocationalCoordinator
</commit_message>
<xml_diff>
--- a/src/assets/templates/Students_Template.xlsx
+++ b/src/assets/templates/Students_Template.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97B0998D-1D2A-4C4C-99F5-6DB54C5D25C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="10500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Students" sheetId="8" r:id="rId1"/>
@@ -15,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="167">
   <si>
     <t>AcademicYear</t>
   </si>
@@ -212,15 +213,9 @@
     <t>varchar(10)</t>
   </si>
   <si>
-    <t>varchar(100)</t>
-  </si>
-  <si>
     <t>DateOfBirth</t>
   </si>
   <si>
-    <t>dd/MM/yyyyy</t>
-  </si>
-  <si>
     <t>Gender</t>
   </si>
   <si>
@@ -233,12 +228,6 @@
     <t>FirstName</t>
   </si>
   <si>
-    <t>AadhaarNumber</t>
-  </si>
-  <si>
-    <t>varchar(12)</t>
-  </si>
-  <si>
     <t>General</t>
   </si>
   <si>
@@ -320,12 +309,6 @@
     <t>DateOfEnrollment</t>
   </si>
   <si>
-    <t>DateOfDropout</t>
-  </si>
-  <si>
-    <t>varchar(20)</t>
-  </si>
-  <si>
     <t>Class 9</t>
   </si>
   <si>
@@ -359,15 +342,6 @@
     <t>Sections</t>
   </si>
   <si>
-    <t>FatherName</t>
-  </si>
-  <si>
-    <t>MotherName</t>
-  </si>
-  <si>
-    <t>GuardianName</t>
-  </si>
-  <si>
     <t>SocialCategory</t>
   </si>
   <si>
@@ -413,41 +387,143 @@
     <t>MobileNumber</t>
   </si>
   <si>
-    <t>FirstMobileNumber</t>
-  </si>
-  <si>
-    <t>SecondMobileNumber</t>
-  </si>
-  <si>
     <t>SchoolName</t>
   </si>
   <si>
-    <t>VTName</t>
-  </si>
-  <si>
-    <t>DropoutReason</t>
-  </si>
-  <si>
-    <t>varchar(250)</t>
-  </si>
-  <si>
-    <t>StudentRollNumber</t>
-  </si>
-  <si>
-    <t>VTEmailId</t>
-  </si>
-  <si>
     <t>UDISE</t>
   </si>
   <si>
     <t>varchar(11)</t>
+  </si>
+  <si>
+    <t>StudentUniqueId</t>
+  </si>
+  <si>
+    <t>JobRole</t>
+  </si>
+  <si>
+    <t>Plumber General</t>
+  </si>
+  <si>
+    <t>Field Technician - Other Home Appliances</t>
+  </si>
+  <si>
+    <t>Sales Associate (New)</t>
+  </si>
+  <si>
+    <t>Food &amp;Beverage Service - Trainee</t>
+  </si>
+  <si>
+    <t>Multiskill Technician (Fabrication)</t>
+  </si>
+  <si>
+    <t>Animator</t>
+  </si>
+  <si>
+    <t>Business Correspondent / Business Facilitator</t>
+  </si>
+  <si>
+    <t>Plumber General II</t>
+  </si>
+  <si>
+    <t>Customer Service Executive (Meet &amp; Greet)</t>
+  </si>
+  <si>
+    <t>Micro Irrigation Technician</t>
+  </si>
+  <si>
+    <t>Home Health Aide</t>
+  </si>
+  <si>
+    <t>Wireman - Control Panel</t>
+  </si>
+  <si>
+    <t>Solanaceous Crop Cultivator</t>
+  </si>
+  <si>
+    <t>Assistant Beauty Therapist</t>
+  </si>
+  <si>
+    <t>Delhi Home</t>
+  </si>
+  <si>
+    <t>Consumer Energy Meter Technician</t>
+  </si>
+  <si>
+    <t>Store Operation Assistant(New)</t>
+  </si>
+  <si>
+    <t>Early Years Physical Activity Facilitator</t>
+  </si>
+  <si>
+    <t>Sewing Machine Operator</t>
+  </si>
+  <si>
+    <t>Beauty Therapist</t>
+  </si>
+  <si>
+    <t>Installation Technician - Computing And Peripherals</t>
+  </si>
+  <si>
+    <t>General Duty Assistant</t>
+  </si>
+  <si>
+    <t>Multiskill Technician Assistant</t>
+  </si>
+  <si>
+    <t>Mulltiskill Wireman - Control Panel</t>
+  </si>
+  <si>
+    <t>Multiskill Micro Irrigation Technician</t>
+  </si>
+  <si>
+    <t>Multiskill Technician (Electrician)</t>
+  </si>
+  <si>
+    <t>Automotive  Service Technician L4</t>
+  </si>
+  <si>
+    <t>Fitness Trainer</t>
+  </si>
+  <si>
+    <t>Delhi Lahi Job</t>
+  </si>
+  <si>
+    <t>Multiskill Technician (Gardnening)</t>
+  </si>
+  <si>
+    <t>SectorName</t>
+  </si>
+  <si>
+    <t>Stream</t>
+  </si>
+  <si>
+    <t>AssessmentToConducted</t>
+  </si>
+  <si>
+    <t>WhatsAppNo</t>
+  </si>
+  <si>
+    <t>Did students have a VE in 9th &amp; 10th?</t>
+  </si>
+  <si>
+    <t>Is the student continuing the same trade?</t>
+  </si>
+  <si>
+    <t>2022-2023</t>
+  </si>
+  <si>
+    <t>2023-2024</t>
+  </si>
+  <si>
+    <t>dd/mm/yyyyy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -489,14 +565,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -518,7 +586,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -541,23 +609,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -576,17 +632,8 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -678,6 +725,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -713,6 +777,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -888,146 +969,126 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="20.77734375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="22" width="14.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>139</v>
-      </c>
       <c r="F1" s="7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>69</v>
+        <v>126</v>
       </c>
       <c r="L1" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>114</v>
+        <v>160</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>116</v>
+        <v>161</v>
       </c>
       <c r="R1" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="S1" s="7" t="s">
-        <v>72</v>
+        <v>108</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>138</v>
+        <v>159</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>117</v>
+        <v>162</v>
       </c>
       <c r="V1" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="W1" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="X1" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="Y1" s="12" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>94</v>
+        <v>125</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>141</v>
+        <v>63</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="E2" s="13" t="s">
         <v>62</v>
       </c>
+      <c r="E2" s="8" t="s">
+        <v>62</v>
+      </c>
       <c r="F2" s="8" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>64</v>
       </c>
       <c r="J2" s="9" t="s">
         <v>64</v>
@@ -1036,31 +1097,31 @@
         <v>63</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="N2" s="9" t="s">
-        <v>67</v>
+      <c r="N2" s="8" t="s">
+        <v>166</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="Q2" s="8" t="s">
-        <v>65</v>
+        <v>62</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>64</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="S2" s="9" t="s">
-        <v>73</v>
+        <v>166</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>62</v>
       </c>
       <c r="T2" s="8" t="s">
-        <v>102</v>
+        <v>62</v>
       </c>
       <c r="U2" s="8" t="s">
         <v>62</v>
@@ -1068,31 +1129,22 @@
       <c r="V2" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="W2" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="X2" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y2" s="9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="6"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
       <c r="G3" s="6"/>
-      <c r="H3" s="10"/>
+      <c r="H3" s="11"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
+      <c r="N3" s="10"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
@@ -1100,26 +1152,23 @@
       <c r="S3" s="11"/>
       <c r="T3" s="11"/>
       <c r="U3" s="11"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="6"/>
+      <c r="V3" s="11"/>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
       <c r="G4" s="6"/>
-      <c r="H4" s="10"/>
+      <c r="H4" s="11"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
+      <c r="N4" s="10"/>
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
@@ -1127,26 +1176,23 @@
       <c r="S4" s="11"/>
       <c r="T4" s="11"/>
       <c r="U4" s="11"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="6"/>
+      <c r="V4" s="11"/>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
       <c r="G5" s="6"/>
-      <c r="H5" s="10"/>
+      <c r="H5" s="11"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
       <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
+      <c r="N5" s="10"/>
       <c r="O5" s="6"/>
       <c r="P5" s="6"/>
       <c r="Q5" s="6"/>
@@ -1154,26 +1200,23 @@
       <c r="S5" s="11"/>
       <c r="T5" s="11"/>
       <c r="U5" s="11"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="6"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="6"/>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="6"/>
+      <c r="V5" s="11"/>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
       <c r="G6" s="6"/>
-      <c r="H6" s="10"/>
+      <c r="H6" s="11"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
+      <c r="N6" s="10"/>
       <c r="O6" s="6"/>
       <c r="P6" s="6"/>
       <c r="Q6" s="6"/>
@@ -1181,26 +1224,23 @@
       <c r="S6" s="11"/>
       <c r="T6" s="11"/>
       <c r="U6" s="11"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="6"/>
+      <c r="V6" s="11"/>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="10"/>
+      <c r="H7" s="11"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
       <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
+      <c r="N7" s="10"/>
       <c r="O7" s="6"/>
       <c r="P7" s="6"/>
       <c r="Q7" s="6"/>
@@ -1208,26 +1248,23 @@
       <c r="S7" s="11"/>
       <c r="T7" s="11"/>
       <c r="U7" s="11"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6"/>
-      <c r="X7" s="6"/>
-      <c r="Y7" s="6"/>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="6"/>
+      <c r="V7" s="11"/>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
       <c r="G8" s="6"/>
-      <c r="H8" s="10"/>
+      <c r="H8" s="11"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="6"/>
-      <c r="N8" s="6"/>
+      <c r="N8" s="10"/>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
       <c r="Q8" s="6"/>
@@ -1235,67 +1272,25 @@
       <c r="S8" s="11"/>
       <c r="T8" s="11"/>
       <c r="U8" s="11"/>
-      <c r="V8" s="6"/>
-      <c r="W8" s="6"/>
-      <c r="X8" s="6"/>
-      <c r="Y8" s="6"/>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="10"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="6"/>
-      <c r="W9" s="6"/>
-      <c r="X9" s="6"/>
-      <c r="Y9" s="6"/>
+      <c r="V8" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Dropdowns!$N$8:$N$10</xm:f>
           </x14:formula1>
-          <xm:sqref>L3:L9</xm:sqref>
+          <xm:sqref>L3:L8</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Dropdowns!$P$9:$P$13</xm:f>
-          </x14:formula1>
-          <xm:sqref>A3:A9</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Dropdowns!$R$9:$R$12</xm:f>
-          </x14:formula1>
-          <xm:sqref>F3:F9</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000003000000}">
           <x14:formula1>
             <xm:f>Dropdowns!$T$9:$T$13</xm:f>
           </x14:formula1>
-          <xm:sqref>G3:G9</xm:sqref>
+          <xm:sqref>G3:G8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1304,38 +1299,38 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:V35"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="B2:V39"/>
   <sheetViews>
-    <sheetView topLeftCell="K7" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="3.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="40.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2.33203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.5546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="8.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="3.33203125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.109375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="17.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="3.5546875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="3.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.140625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="17.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="3.5703125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.85546875" style="2" customWidth="1"/>
     <col min="16" max="16" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="4.109375" style="2" customWidth="1"/>
-    <col min="18" max="18" width="25.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.44140625" style="2" customWidth="1"/>
-    <col min="20" max="20" width="26.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="3.33203125" style="2" customWidth="1"/>
-    <col min="22" max="22" width="52.6640625" style="2" customWidth="1"/>
-    <col min="23" max="16384" width="9.109375" style="2"/>
+    <col min="17" max="17" width="4.140625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="25.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.42578125" style="2" customWidth="1"/>
+    <col min="20" max="20" width="26.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="3.28515625" style="2" customWidth="1"/>
+    <col min="22" max="22" width="52.7109375" style="2" customWidth="1"/>
+    <col min="23" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:22" x14ac:dyDescent="0.2">
@@ -1361,19 +1356,19 @@
         <v>1</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="V2" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="2:22" ht="14.4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:22" ht="15" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>3</v>
       </c>
@@ -1396,19 +1391,19 @@
         <v>58</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="R3" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="T3" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="T3" s="5" t="s">
-        <v>84</v>
-      </c>
       <c r="V3" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="4" spans="2:22" ht="14.4" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" ht="15" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1431,19 +1426,19 @@
         <v>59</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="R4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="T4" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="T4" s="5" t="s">
-        <v>85</v>
-      </c>
       <c r="V4" s="5" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="2:22" ht="14.4" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" ht="15" x14ac:dyDescent="0.2">
       <c r="F5" s="5" t="s">
         <v>10</v>
       </c>
@@ -1460,19 +1455,19 @@
         <v>60</v>
       </c>
       <c r="P5" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="R5" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="T5" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="T5" s="5" t="s">
-        <v>86</v>
-      </c>
       <c r="V5" s="5" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="6" spans="2:22" ht="14.4" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" ht="15" x14ac:dyDescent="0.2">
       <c r="F6" s="5" t="s">
         <v>11</v>
       </c>
@@ -1486,19 +1481,19 @@
         <v>29</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="R6" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="T6" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="T6" s="5" t="s">
-        <v>87</v>
-      </c>
       <c r="V6" s="5" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="2:22" ht="14.4" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" ht="15" x14ac:dyDescent="0.2">
       <c r="F7" s="5" t="s">
         <v>12</v>
       </c>
@@ -1510,64 +1505,76 @@
         <v>30</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="V7" s="5" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="2:22" ht="14.4" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" ht="15" x14ac:dyDescent="0.2">
+      <c r="F8" s="3" t="s">
+        <v>164</v>
+      </c>
       <c r="L8" s="5" t="s">
         <v>31</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="P8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="R8" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="T8" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="T8" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="2:22" ht="14.4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="2:22" ht="15" x14ac:dyDescent="0.2">
+      <c r="F9" s="3" t="s">
+        <v>165</v>
+      </c>
       <c r="L9" s="5" t="s">
         <v>32</v>
       </c>
       <c r="N9" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="P9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="2:22" ht="14.4" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L10" s="5" t="s">
         <v>33</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="P10" s="5" t="s">
         <v>11</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="T10" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="11" spans="2:22" ht="14.4" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="V10" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L11" s="5" t="s">
         <v>34</v>
       </c>
@@ -1575,196 +1582,294 @@
         <v>9</v>
       </c>
       <c r="R11" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="T11" s="5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="12" spans="2:22" ht="14.4" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="V11" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L12" s="5" t="s">
         <v>35</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="P12" s="5" t="s">
         <v>10</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="T12" s="5" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="13" spans="2:22" ht="14.4" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="V12" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L13" s="5" t="s">
         <v>36</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="P13" s="5" t="s">
         <v>12</v>
       </c>
       <c r="T13" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="2:22" ht="14.4" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="V13" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="2:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L14" s="5" t="s">
         <v>37</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="2:22" ht="14.4" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="V14" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="2:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L15" s="5" t="s">
         <v>38</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="16" spans="2:22" ht="14.4" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+      <c r="V15" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L16" s="5" t="s">
         <v>39</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="P16" s="5" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="17" spans="12:16" ht="14.4" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="12:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L17" s="5" t="s">
         <v>40</v>
       </c>
       <c r="P17" s="5" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="18" spans="12:16" ht="14.4" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+      <c r="V17" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="12:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L18" s="5" t="s">
         <v>41</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="19" spans="12:16" ht="14.4" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+      <c r="V18" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="19" spans="12:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L19" s="5" t="s">
         <v>42</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="20" spans="12:16" ht="14.4" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="V19" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="12:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L20" s="5" t="s">
         <v>19</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="21" spans="12:16" ht="14.4" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+      <c r="V20" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="21" spans="12:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L21" s="5" t="s">
         <v>43</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="22" spans="12:16" ht="14.4" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+      <c r="V21" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="12:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L22" s="5" t="s">
         <v>44</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="23" spans="12:16" ht="14.4" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+      <c r="V22" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="23" spans="12:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L23" s="5" t="s">
         <v>45</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="24" spans="12:16" ht="14.4" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+      <c r="V23" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="12:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L24" s="5" t="s">
         <v>46</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="25" spans="12:16" ht="14.4" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+      <c r="V24" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="25" spans="12:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L25" s="5" t="s">
         <v>47</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="26" spans="12:16" ht="14.4" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="V25" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="12:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L26" s="5" t="s">
         <v>48</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="27" spans="12:16" ht="14.4" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+      <c r="V26" s="3" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="27" spans="12:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L27" s="5" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="28" spans="12:16" ht="14.4" x14ac:dyDescent="0.2">
+      <c r="V27" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="28" spans="12:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L28" s="5" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="29" spans="12:16" ht="14.4" x14ac:dyDescent="0.2">
+      <c r="V28" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="29" spans="12:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L29" s="5" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="30" spans="12:16" ht="14.4" x14ac:dyDescent="0.2">
+      <c r="V29" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="30" spans="12:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L30" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="31" spans="12:16" ht="14.4" x14ac:dyDescent="0.2">
+      <c r="V30" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="31" spans="12:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L31" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="32" spans="12:16" ht="14.4" x14ac:dyDescent="0.2">
+      <c r="V31" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="32" spans="12:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L32" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="33" spans="12:12" ht="14.4" x14ac:dyDescent="0.2">
+      <c r="V32" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="12:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L33" s="5" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="34" spans="12:12" ht="14.4" x14ac:dyDescent="0.2">
+      <c r="V33" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="12:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L34" s="5" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="35" spans="12:12" ht="14.4" x14ac:dyDescent="0.2">
+      <c r="V34" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="12:22" ht="15" x14ac:dyDescent="0.2">
       <c r="L35" s="5" t="s">
         <v>57</v>
+      </c>
+      <c r="V35" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="V36" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="37" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="V37" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="V38" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="39" spans="12:22" x14ac:dyDescent="0.2">
+      <c r="V39" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>